<commit_message>
ProgressiveAutomation after completing UI
</commit_message>
<xml_diff>
--- a/src/main/resources/data/TestData.xlsx
+++ b/src/main/resources/data/TestData.xlsx
@@ -8,13 +8,16 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Nista Shrestha\IdeaProjects\ProgressiveAutomation\src\main\resources\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9BDB4FF9-048D-470D-992A-254596AD342C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A2DE0E89-1054-4726-96FA-F91736396BD0}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-98" yWindow="-98" windowWidth="21795" windowHeight="13096" activeTab="1" xr2:uid="{8177844E-082B-4792-A4CF-6F379A0FF935}"/>
+    <workbookView xWindow="-98" yWindow="-98" windowWidth="21795" windowHeight="13096" activeTab="4" xr2:uid="{8177844E-082B-4792-A4CF-6F379A0FF935}"/>
   </bookViews>
   <sheets>
     <sheet name="personalInfo" sheetId="1" r:id="rId1"/>
     <sheet name="vehicleInfo" sheetId="2" r:id="rId2"/>
+    <sheet name="removeVehicle" sheetId="3" r:id="rId3"/>
+    <sheet name="driverInformation" sheetId="4" r:id="rId4"/>
+    <sheet name="AdditionalDetail" sheetId="5" r:id="rId5"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -35,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="72" uniqueCount="59">
   <si>
     <t>enterFirstName</t>
   </si>
@@ -106,20 +109,136 @@
     <t>5</t>
   </si>
   <si>
-    <t>CX-7</t>
-  </si>
-  <si>
-    <t>SUV (4CYL 4x2)</t>
+    <t>null</t>
+  </si>
+  <si>
+    <t>2012</t>
+  </si>
+  <si>
+    <t>BMW</t>
+  </si>
+  <si>
+    <t>328</t>
+  </si>
+  <si>
+    <t>2DR 6CYL</t>
+  </si>
+  <si>
+    <t>2014</t>
+  </si>
+  <si>
+    <t>Kia</t>
+  </si>
+  <si>
+    <t>Forte</t>
+  </si>
+  <si>
+    <t>2DR 4CYL</t>
+  </si>
+  <si>
+    <t>gender</t>
+  </si>
+  <si>
+    <t>selectMaritalStatus</t>
+  </si>
+  <si>
+    <t>selectEducation</t>
+  </si>
+  <si>
+    <t>selectEmployment</t>
+  </si>
+  <si>
+    <t>socialSecurityNumber</t>
+  </si>
+  <si>
+    <t>primaryResidency</t>
+  </si>
+  <si>
+    <t>hasPriorAddress</t>
+  </si>
+  <si>
+    <t>licensed</t>
+  </si>
+  <si>
+    <t>accident</t>
+  </si>
+  <si>
+    <t>ticket</t>
+  </si>
+  <si>
+    <t>Female</t>
+  </si>
+  <si>
+    <t>Single</t>
+  </si>
+  <si>
+    <t>College degree</t>
+  </si>
+  <si>
+    <t>Employed</t>
+  </si>
+  <si>
+    <t>enterOccupation</t>
+  </si>
+  <si>
+    <t>Quality Assurance Tester</t>
+  </si>
+  <si>
+    <t>Own home</t>
+  </si>
+  <si>
+    <t>No</t>
+  </si>
+  <si>
+    <t>At least 2 years, but less than 3 years</t>
+  </si>
+  <si>
+    <t>insuranceToday</t>
+  </si>
+  <si>
+    <t>insuranceLastMonth</t>
+  </si>
+  <si>
+    <t>nonAutoPolicy</t>
+  </si>
+  <si>
+    <t>emailAddress</t>
+  </si>
+  <si>
+    <t>totalResident</t>
+  </si>
+  <si>
+    <t>residence</t>
+  </si>
+  <si>
+    <t>stha@gmail.com</t>
+  </si>
+  <si>
+    <t>Less than 1 year</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="8"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -142,15 +261,18 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -525,7 +647,244 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D45527F6-37E6-496D-B07E-344EC7BDA67C}">
-  <dimension ref="A1:G3"/>
+  <dimension ref="A1:G4"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D32" sqref="D32"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <cols>
+    <col min="4" max="4" width="12.86328125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="42.33203125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="12.796875" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="21.06640625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="13.86328125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A1" t="s">
+        <v>10</v>
+      </c>
+      <c r="B1" t="s">
+        <v>11</v>
+      </c>
+      <c r="C1" t="s">
+        <v>12</v>
+      </c>
+      <c r="D1" t="s">
+        <v>13</v>
+      </c>
+      <c r="E1" t="s">
+        <v>14</v>
+      </c>
+      <c r="F1" t="s">
+        <v>15</v>
+      </c>
+      <c r="G1" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A2" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="B2" t="s">
+        <v>21</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="D2" t="s">
+        <v>23</v>
+      </c>
+      <c r="E2" t="s">
+        <v>17</v>
+      </c>
+      <c r="F2" t="s">
+        <v>18</v>
+      </c>
+      <c r="G2" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A3" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="B3" t="s">
+        <v>25</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="D3" t="s">
+        <v>27</v>
+      </c>
+      <c r="E3" t="s">
+        <v>17</v>
+      </c>
+      <c r="F3" t="s">
+        <v>18</v>
+      </c>
+      <c r="G3" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A4" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="B4" t="s">
+        <v>29</v>
+      </c>
+      <c r="C4" t="s">
+        <v>30</v>
+      </c>
+      <c r="D4" t="s">
+        <v>31</v>
+      </c>
+      <c r="E4" t="s">
+        <v>17</v>
+      </c>
+      <c r="F4" t="s">
+        <v>18</v>
+      </c>
+      <c r="G4" t="s">
+        <v>19</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="1" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{675C0455-E62B-4FE0-B832-87237B61690B}">
+  <dimension ref="A1:A2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetData>
+    <row r="1" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A1" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A2" t="s">
+        <v>25</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1FCFFD21-8F33-4688-AED5-B3D62CC7FAA0}">
+  <dimension ref="A1:K2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <cols>
+    <col min="2" max="2" width="16" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="13.1328125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="15.265625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="20.33203125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="17.9296875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="14.73046875" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="13.46484375" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="30.19921875" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:11" x14ac:dyDescent="0.45">
+      <c r="A1" t="s">
+        <v>32</v>
+      </c>
+      <c r="B1" t="s">
+        <v>33</v>
+      </c>
+      <c r="C1" t="s">
+        <v>34</v>
+      </c>
+      <c r="D1" t="s">
+        <v>35</v>
+      </c>
+      <c r="E1" t="s">
+        <v>46</v>
+      </c>
+      <c r="F1" t="s">
+        <v>36</v>
+      </c>
+      <c r="G1" t="s">
+        <v>37</v>
+      </c>
+      <c r="H1" t="s">
+        <v>38</v>
+      </c>
+      <c r="I1" t="s">
+        <v>39</v>
+      </c>
+      <c r="J1" t="s">
+        <v>40</v>
+      </c>
+      <c r="K1" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11" x14ac:dyDescent="0.45">
+      <c r="A2" t="s">
+        <v>42</v>
+      </c>
+      <c r="B2" t="s">
+        <v>43</v>
+      </c>
+      <c r="C2" t="s">
+        <v>44</v>
+      </c>
+      <c r="D2" t="s">
+        <v>45</v>
+      </c>
+      <c r="E2" t="s">
+        <v>47</v>
+      </c>
+      <c r="F2">
+        <v>123456789</v>
+      </c>
+      <c r="G2" t="s">
+        <v>48</v>
+      </c>
+      <c r="H2" t="s">
+        <v>49</v>
+      </c>
+      <c r="I2" t="s">
+        <v>50</v>
+      </c>
+      <c r="J2" t="s">
+        <v>49</v>
+      </c>
+      <c r="K2" t="s">
+        <v>49</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BA55D200-808C-4C3A-9D09-86D1B9ABE017}">
+  <dimension ref="A1:F2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="A2" sqref="A2"/>
@@ -533,83 +892,58 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="4" max="4" width="12.86328125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="42.33203125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="12.796875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="13.06640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="16.86328125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="12.1328125" bestFit="1" customWidth="1"/>
+    <col min="4" max="5" width="11.265625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="13.3984375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A1" t="s">
-        <v>10</v>
+        <v>51</v>
       </c>
       <c r="B1" t="s">
-        <v>11</v>
+        <v>52</v>
       </c>
       <c r="C1" t="s">
-        <v>12</v>
+        <v>53</v>
       </c>
       <c r="D1" t="s">
-        <v>13</v>
+        <v>54</v>
       </c>
       <c r="E1" t="s">
-        <v>14</v>
+        <v>55</v>
       </c>
       <c r="F1" t="s">
-        <v>15</v>
-      </c>
-      <c r="G1" t="s">
-        <v>16</v>
+        <v>56</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.45">
-      <c r="A2" s="2" t="s">
-        <v>20</v>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A2" t="s">
+        <v>49</v>
       </c>
       <c r="B2" t="s">
-        <v>21</v>
-      </c>
-      <c r="C2" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="D2">
-        <v>0</v>
-      </c>
-      <c r="E2" t="s">
-        <v>17</v>
+        <v>49</v>
+      </c>
+      <c r="C2" t="s">
+        <v>49</v>
+      </c>
+      <c r="D2" s="3" t="s">
+        <v>57</v>
+      </c>
+      <c r="E2">
+        <v>1</v>
       </c>
       <c r="F2" t="s">
-        <v>18</v>
-      </c>
-      <c r="G2" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.45">
-      <c r="A3" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="B3" t="s">
-        <v>21</v>
-      </c>
-      <c r="C3" s="2" t="s">
-        <v>23</v>
-      </c>
-      <c r="D3" t="s">
-        <v>24</v>
-      </c>
-      <c r="E3" t="s">
-        <v>17</v>
-      </c>
-      <c r="F3" t="s">
-        <v>18</v>
-      </c>
-      <c r="G3" t="s">
-        <v>19</v>
+        <v>58</v>
       </c>
     </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="D2" r:id="rId1" xr:uid="{474CF1FE-101A-45FD-888E-661681B31C06}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -799,18 +1133,18 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
 <FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
   <Display>DocumentLibraryForm</Display>
   <Edit>DocumentLibraryForm</Edit>
   <New>DocumentLibraryForm</New>
 </FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -833,6 +1167,14 @@
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{21536B71-219D-49CD-9128-CC1101C59450}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{2669F683-8FF9-4723-A317-47DA32DBE2B0}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="56caf978-ed08-4319-8660-ea565c3c81d4"/>
@@ -847,12 +1189,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{21536B71-219D-49CD-9128-CC1101C59450}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>